<commit_message>
Se añade el documento de la tarea
</commit_message>
<xml_diff>
--- a/Practica01 ordenamientos/graficasP01.xlsx
+++ b/Practica01 ordenamientos/graficasP01.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iAngelMx\Documents\GitHub\algorithmAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GITS\algorithmAnalysis\Practica01 ordenamientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{61A11520-7DA6-487D-AA43-1C556185FCAE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EE782B3-B11B-4EA1-A3AE-8414B9BE15C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{C11530CD-E7D9-4FCE-9D0E-7C319F9665DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1493,6 +1490,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Número de datos insertados a ordenar</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1558,6 +1610,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Segundos de ejecución</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1690,25 +1797,21 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="es-MX"/>
-              <a:t>Bubble</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-MX" baseline="0"/>
-              <a:t> sort</a:t>
+              <a:t>Bubble sort</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1726,16 +1829,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="es-MX"/>
@@ -1763,7 +1866,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1865,7 +1968,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1971,6 +2074,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Raíz cuadrada de la cantidad de datos insertados</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1993,7 +2151,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2036,6 +2194,75 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Segundos de ejecución</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2080,7 +2307,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2744,7 +2971,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2755,7 +2982,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2778,14 +3005,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2801,7 +3028,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2821,22 +3048,17 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2845,12 +3067,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2860,12 +3082,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2877,13 +3099,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="38100" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2892,36 +3114,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2943,15 +3158,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2966,15 +3179,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2985,17 +3198,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3004,14 +3217,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3023,21 +3236,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3056,7 +3263,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3075,17 +3282,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3094,17 +3301,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3125,7 +3331,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -3133,7 +3339,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3146,6 +3352,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3153,10 +3370,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -3171,13 +3388,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3186,14 +3403,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3223,8 +3440,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3247,14 +3464,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3300,15 +3511,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>104774</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3334,185 +3545,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="salida"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Tiempo de ejecución</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>80</v>
-          </cell>
-          <cell r="B2">
-            <v>5.0010000000000002E-3</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>160</v>
-          </cell>
-          <cell r="B3">
-            <v>1.5003000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>240</v>
-          </cell>
-          <cell r="B4">
-            <v>3.7007999999999999E-2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>320</v>
-          </cell>
-          <cell r="B5">
-            <v>5.2006999999999998E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>400</v>
-          </cell>
-          <cell r="B6">
-            <v>7.4476000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>480</v>
-          </cell>
-          <cell r="B7">
-            <v>0.135042</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>560</v>
-          </cell>
-          <cell r="B8">
-            <v>0.163053</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>640</v>
-          </cell>
-          <cell r="B9">
-            <v>0.24954899999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>720</v>
-          </cell>
-          <cell r="B10">
-            <v>0.304062</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>800</v>
-          </cell>
-          <cell r="B11">
-            <v>0.32103999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>880</v>
-          </cell>
-          <cell r="B12">
-            <v>0.35905399999999998</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>960</v>
-          </cell>
-          <cell r="B13">
-            <v>0.469084</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>1040</v>
-          </cell>
-          <cell r="B14">
-            <v>0.54307000000000005</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>1120</v>
-          </cell>
-          <cell r="B15">
-            <v>0.58905200000000002</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>1200</v>
-          </cell>
-          <cell r="B16">
-            <v>0.71509999999999996</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>1280</v>
-          </cell>
-          <cell r="B17">
-            <v>0.73909100000000005</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>1360</v>
-          </cell>
-          <cell r="B18">
-            <v>0.86658999999999997</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>1440</v>
-          </cell>
-          <cell r="B19">
-            <v>1.1366700000000001</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>1520</v>
-          </cell>
-          <cell r="B20">
-            <v>1.1271359999999999</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>1600</v>
-          </cell>
-          <cell r="B21">
-            <v>1.34117</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3814,8 +3846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E4D422-3B30-4F02-BAB2-658AAA00FA23}">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="N102" sqref="N102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>